<commit_message>
Documentation and Diagramme updated Concept more or less finished
</commit_message>
<xml_diff>
--- a/Doc/CurveRule.xlsx
+++ b/Doc/CurveRule.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sascha\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Google Drive\Projects\nepo\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -116,6 +116,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Zielfunktion der</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" baseline="0"/>
+              <a:t> Kommunen</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -148,16 +178,19 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Phase 1</c:v>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -166,7 +199,94 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$3:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Tabelle1!$G$3:$G$28</c:f>
               <c:numCache>
@@ -252,7 +372,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -263,8 +383,11 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Phase 2</c:v>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -275,7 +398,94 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$3:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Tabelle1!$F$3:$F$28</c:f>
               <c:numCache>
@@ -361,7 +571,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -372,8 +582,11 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Phase 3</c:v>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -384,7 +597,94 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$3:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Tabelle1!$E$3:$E$28</c:f>
               <c:numCache>
@@ -470,7 +770,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -481,8 +781,11 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:v>Phase 4</c:v>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -493,7 +796,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Tabelle1!$C$3:$C$28</c:f>
               <c:numCache>
@@ -579,8 +882,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Tabelle1!$D$3:$D$28</c:f>
               <c:numCache>
@@ -666,11 +969,123 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-DA9F-47D6-8DE3-0CE1EB537EBD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Min</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$8:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$10:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-37E2-422E-B743-03998BABB515}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Max</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$9:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$10:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-37E2-422E-B743-03998BABB515}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -682,20 +1097,74 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="1457770400"/>
         <c:axId val="1391166816"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="1457770400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Enternung vom Sendemast</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -732,15 +1201,16 @@
         </c:txPr>
         <c:crossAx val="1391166816"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+        <c:minorUnit val="2"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="1391166816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.5"/>
+          <c:min val="-1.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -758,6 +1228,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Wert der Zielfunktion</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -791,7 +1316,7 @@
         </c:txPr>
         <c:crossAx val="1457770400"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -801,8 +1326,39 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1398,16 +1954,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>328612</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:rowOff>147636</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>328612</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1734,13 +2290,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:F28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E2">
         <v>0.2</v>
       </c>
@@ -1751,7 +2307,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1778,7 +2334,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1805,7 +2361,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <f>(B4-B3)/2</f>
         <v>4.5</v>
@@ -1830,7 +2386,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>1.5</v>
       </c>
@@ -1851,7 +2407,7 @@
         <v>-0.95555555555555549</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>2</v>
       </c>
@@ -1872,7 +2428,15 @@
         <v>-0.89876543209876547</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f>B3</f>
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <f>B3</f>
+        <v>3</v>
+      </c>
       <c r="C8">
         <v>2.5</v>
       </c>
@@ -1893,7 +2457,15 @@
         <v>-0.84691358024691366</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f>B4</f>
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <f>B4</f>
+        <v>12</v>
+      </c>
       <c r="C9">
         <v>3</v>
       </c>
@@ -1914,7 +2486,13 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>-2</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
       <c r="C10">
         <v>3.5</v>
       </c>
@@ -1935,7 +2513,7 @@
         <v>0.84197530864197534</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>4</v>
       </c>
@@ -1956,7 +2534,7 @@
         <v>0.87901234567901243</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>4.5</v>
       </c>
@@ -1977,7 +2555,7 @@
         <v>0.9111111111111112</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>5</v>
       </c>
@@ -1998,7 +2576,7 @@
         <v>0.93827160493827155</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>5.5</v>
       </c>
@@ -2019,7 +2597,7 @@
         <v>0.96049382716049381</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>6</v>
       </c>
@@ -2040,7 +2618,7 @@
         <v>0.97777777777777775</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>6.5</v>
       </c>
@@ -2061,7 +2639,7 @@
         <v>0.99012345679012348</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>7</v>
       </c>
@@ -2082,7 +2660,7 @@
         <v>0.9975308641975309</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>7.5</v>
       </c>
@@ -2103,7 +2681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C19">
         <v>8</v>
       </c>
@@ -2124,7 +2702,7 @@
         <v>0.9975308641975309</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>8.5</v>
       </c>
@@ -2145,7 +2723,7 @@
         <v>0.99012345679012348</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>9</v>
       </c>
@@ -2166,7 +2744,7 @@
         <v>0.97777777777777775</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>9.5</v>
       </c>
@@ -2187,7 +2765,7 @@
         <v>0.96049382716049381</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>10</v>
       </c>
@@ -2208,7 +2786,7 @@
         <v>0.93827160493827155</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>10.5</v>
       </c>
@@ -2229,7 +2807,7 @@
         <v>0.9111111111111112</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>11</v>
       </c>
@@ -2250,7 +2828,7 @@
         <v>0.87901234567901243</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>11.5</v>
       </c>
@@ -2271,7 +2849,7 @@
         <v>0.84197530864197534</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>12</v>
       </c>
@@ -2292,7 +2870,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>12.5</v>
       </c>

</xml_diff>